<commit_message>
feat: exclusão de planlhas desnecessárias
</commit_message>
<xml_diff>
--- a/geometria_da_sapata (2).xlsx
+++ b/geometria_da_sapata (2).xlsx
@@ -452,10 +452,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>2.633597347071823</v>
+        <v>4.33631436872199</v>
       </c>
       <c r="B2" t="n">
-        <v>2.659562300241746</v>
+        <v>2.559828710052578</v>
       </c>
       <c r="C2" t="n">
         <v>0.6</v>
@@ -463,10 +463,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1.929113309454846</v>
+        <v>3.104068870015793</v>
       </c>
       <c r="B3" t="n">
-        <v>4.991604021980758</v>
+        <v>1.1354757379688</v>
       </c>
       <c r="C3" t="n">
         <v>0.6</v>
@@ -474,10 +474,10 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>2.126807295539599</v>
+        <v>1.062341570308431</v>
       </c>
       <c r="B4" t="n">
-        <v>4.94182926912892</v>
+        <v>1.435495356548319</v>
       </c>
       <c r="C4" t="n">
         <v>0.6</v>
@@ -485,10 +485,10 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>3.256024836657743</v>
+        <v>1.653148343425738</v>
       </c>
       <c r="B5" t="n">
-        <v>0.9952275742670242</v>
+        <v>2.786676407812485</v>
       </c>
       <c r="C5" t="n">
         <v>0.6</v>
@@ -496,10 +496,10 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>3.999989404163209</v>
+        <v>2.738549572119815</v>
       </c>
       <c r="B6" t="n">
-        <v>3.834512800877488</v>
+        <v>4.512419884876583</v>
       </c>
       <c r="C6" t="n">
         <v>0.6</v>

</xml_diff>